<commit_message>
Changes required to update Australia scaling inventory
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Australia_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Australia_scaling_mapping.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/mappings/scaling/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB58DFF-A9E3-2740-97F4-B04C3F765608}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16060" yWindow="7560" windowWidth="17340" windowHeight="12980" activeTab="2"/>
+    <workbookView xWindow="11460" yWindow="5020" windowWidth="17340" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="219">
   <si>
     <t>iso</t>
   </si>
@@ -666,12 +672,24 @@
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>Other Administrative Services [729]</t>
+  </si>
+  <si>
+    <t>Air and Space Transport [490]</t>
+  </si>
+  <si>
+    <t>Iron and Steel Forging [221]</t>
+  </si>
+  <si>
+    <t>Pump, Compressor, Heating and Ventilation Equipment Manufacturing [245]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1383,29 +1401,29 @@
   </cellXfs>
   <cellStyles count="175">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="47"/>
+    <cellStyle name="20% - Accent1 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="49"/>
+    <cellStyle name="20% - Accent2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="51"/>
+    <cellStyle name="20% - Accent3 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="53"/>
+    <cellStyle name="20% - Accent4 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="55"/>
+    <cellStyle name="20% - Accent5 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="57"/>
+    <cellStyle name="20% - Accent6 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="48"/>
+    <cellStyle name="40% - Accent1 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="50"/>
+    <cellStyle name="40% - Accent2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="52"/>
+    <cellStyle name="40% - Accent3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="54"/>
+    <cellStyle name="40% - Accent4 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="56"/>
+    <cellStyle name="40% - Accent5 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="58"/>
+    <cellStyle name="40% - Accent6 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
@@ -1547,12 +1565,12 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="43"/>
-    <cellStyle name="Normal 3" xfId="45"/>
-    <cellStyle name="Normal 4" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="43" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Normal 3" xfId="45" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Normal 4" xfId="42" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note 2" xfId="44"/>
-    <cellStyle name="Note 3" xfId="46"/>
+    <cellStyle name="Note 2" xfId="44" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Note 3" xfId="46" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
@@ -1563,6 +1581,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1854,23 +1875,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J156"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B141" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A74" sqref="A74"/>
+      <selection pane="bottomRight" activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="1" max="1" width="50.6640625" customWidth="1"/>
     <col min="2" max="2" width="35.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
@@ -1887,7 +1908,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1898,7 +1919,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1909,7 +1930,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>26</v>
       </c>
@@ -1920,7 +1941,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
@@ -1928,7 +1949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
@@ -1936,7 +1957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -1944,7 +1965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>34</v>
       </c>
@@ -1952,7 +1973,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>39</v>
       </c>
@@ -1960,7 +1981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>49</v>
       </c>
@@ -1968,7 +1989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
         <v>52</v>
       </c>
@@ -1976,7 +1997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
         <v>103</v>
       </c>
@@ -1984,7 +2005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
         <v>94</v>
       </c>
@@ -1992,7 +2013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
         <v>95</v>
       </c>
@@ -2000,7 +2021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -2008,15 +2029,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
         <v>101</v>
       </c>
@@ -2024,7 +2045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
         <v>87</v>
       </c>
@@ -2032,7 +2053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
         <v>86</v>
       </c>
@@ -2040,7 +2061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
         <v>133</v>
       </c>
@@ -2048,7 +2069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="28" customFormat="1">
+    <row r="21" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
         <v>93</v>
       </c>
@@ -2056,7 +2077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="28" customFormat="1">
+    <row r="22" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
         <v>127</v>
       </c>
@@ -2064,7 +2085,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="28" customFormat="1">
+    <row r="23" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
         <v>65</v>
       </c>
@@ -2072,7 +2093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="28" customFormat="1">
+    <row r="24" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
         <v>151</v>
       </c>
@@ -2080,7 +2101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="28" customFormat="1">
+    <row r="25" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
         <v>118</v>
       </c>
@@ -2088,7 +2109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2096,7 +2117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
         <v>134</v>
       </c>
@@ -2104,7 +2125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="28" t="s">
         <v>139</v>
       </c>
@@ -2113,7 +2134,7 @@
       </c>
       <c r="J28" s="28"/>
     </row>
-    <row r="29" spans="1:10" s="10" customFormat="1">
+    <row r="29" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="28" t="s">
         <v>124</v>
       </c>
@@ -2123,7 +2144,7 @@
       <c r="F29"/>
       <c r="J29" s="28"/>
     </row>
-    <row r="30" spans="1:10" s="28" customFormat="1">
+    <row r="30" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -2131,7 +2152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="28" customFormat="1">
+    <row r="31" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -2139,7 +2160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -2148,7 +2169,7 @@
       </c>
       <c r="J32" s="28"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
         <v>130</v>
       </c>
@@ -2157,7 +2178,7 @@
       </c>
       <c r="J33" s="28"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -2166,384 +2187,368 @@
       </c>
       <c r="J34" s="28"/>
     </row>
-    <row r="35" spans="1:10" s="28" customFormat="1"/>
-    <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="16" t="s">
+    <row r="35" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B38" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C38" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="J36" s="28"/>
-    </row>
-    <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="16" t="s">
+      <c r="F38" s="10"/>
+      <c r="J38" s="28"/>
+    </row>
+    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="B37" s="63" t="s">
-        <v>200</v>
-      </c>
-      <c r="C37" s="43"/>
-      <c r="F37" s="16"/>
-      <c r="J37" s="28"/>
-    </row>
-    <row r="38" spans="1:10" ht="15">
-      <c r="A38" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="63" t="s">
-        <v>200</v>
-      </c>
-      <c r="J38" s="28"/>
-    </row>
-    <row r="39" spans="1:10" ht="15">
-      <c r="A39" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="B39" s="63" t="s">
         <v>200</v>
       </c>
-      <c r="C39" s="10"/>
-    </row>
-    <row r="40" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A40" s="16"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="16"/>
-    </row>
-    <row r="41" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A41" s="9" t="s">
+      <c r="C39" s="43"/>
+      <c r="F39" s="16"/>
+      <c r="J39" s="28"/>
+    </row>
+    <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="63" t="s">
+        <v>200</v>
+      </c>
+      <c r="J40" s="28"/>
+    </row>
+    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="63" t="s">
+        <v>200</v>
+      </c>
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="16"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="16"/>
+    </row>
+    <row r="43" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B43" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="54" t="s">
+      <c r="C43" s="54" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="10" customFormat="1" ht="15">
-      <c r="A42" s="13" t="s">
+    <row r="44" spans="1:10" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="J42" s="28"/>
-    </row>
-    <row r="43" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A43" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="45" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A44" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="B44" s="34" t="s">
         <v>19</v>
       </c>
       <c r="C44" s="45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A45" s="28" t="s">
-        <v>135</v>
+        <v>169</v>
+      </c>
+      <c r="J44" s="28"/>
+    </row>
+    <row r="45" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="B45" s="34" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A46" s="28" t="s">
-        <v>136</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="B46" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="C46" s="45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B47" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="10"/>
-    </row>
-    <row r="48" spans="1:10" s="28" customFormat="1" ht="15">
+      <c r="C47" s="45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="28" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B48" s="34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15">
+    <row r="49" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="28" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="B49" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="28"/>
-    </row>
-    <row r="50" spans="1:10" ht="15">
+      <c r="C49" s="10"/>
+    </row>
+    <row r="50" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="28" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B50" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="28"/>
-    </row>
-    <row r="51" spans="1:10" ht="15">
+    </row>
+    <row r="51" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="28" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B51" s="34" t="s">
         <v>19</v>
       </c>
       <c r="C51" s="28"/>
     </row>
-    <row r="52" spans="1:10" ht="15">
-      <c r="A52" t="s">
+    <row r="52" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="28"/>
+    </row>
+    <row r="53" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="28"/>
+    </row>
+    <row r="54" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>119</v>
-      </c>
-      <c r="B52" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" s="28"/>
-    </row>
-    <row r="53" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A53" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="15">
-      <c r="A54" s="28" t="s">
-        <v>150</v>
       </c>
       <c r="B54" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="J54" s="28"/>
-    </row>
-    <row r="55" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A55" t="s">
-        <v>76</v>
+      <c r="C54" s="28"/>
+    </row>
+    <row r="55" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="B55" s="38" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15">
+    <row r="56" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B56" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="28"/>
-    </row>
-    <row r="57" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A57" s="28" t="s">
-        <v>70</v>
+      <c r="J56" s="28"/>
+    </row>
+    <row r="57" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>76</v>
       </c>
       <c r="B57" s="38" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A58" t="s">
-        <v>84</v>
-      </c>
-      <c r="B58" s="38" t="s">
+    <row r="58" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A59" t="s">
-        <v>111</v>
+      <c r="C58" s="28"/>
+    </row>
+    <row r="59" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="28" t="s">
+        <v>70</v>
       </c>
       <c r="B59" s="38" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="28" customFormat="1" ht="15">
+    <row r="60" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B60" s="38" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
-      <c r="J62" s="28"/>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="2" t="s">
+    <row r="61" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J64" s="28"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B65" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="C63" s="59" t="s">
+      <c r="C65" s="59" t="s">
         <v>195</v>
       </c>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="28"/>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="2" t="s">
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B64" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="D64" s="28"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="28"/>
-      <c r="H64" s="28"/>
-      <c r="I64" s="28"/>
-      <c r="J64" s="28"/>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="B65" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="G65" s="21"/>
-    </row>
-    <row r="66" spans="1:10" s="28" customFormat="1">
-      <c r="A66" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="B66" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
-    </row>
-    <row r="67" spans="1:10" s="28" customFormat="1">
-      <c r="A67" t="s">
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="28"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="G67" s="21"/>
+    </row>
+    <row r="68" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
+      <c r="H68"/>
+      <c r="I68"/>
+    </row>
+    <row r="69" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>104</v>
       </c>
-      <c r="B67" s="39" t="s">
+      <c r="B69" s="39" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
-      <c r="A68" t="s">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>146</v>
       </c>
-      <c r="B68" s="62" t="s">
+      <c r="B70" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="C68" s="28"/>
-    </row>
-    <row r="69" spans="1:10" s="28" customFormat="1">
-      <c r="B69" s="62"/>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="11" t="s">
+      <c r="C70" s="28"/>
+    </row>
+    <row r="71" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="62"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="31" t="s">
+      <c r="B72" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="C70" s="60" t="s">
+      <c r="C72" s="60" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
-      <c r="A71" t="s">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>144</v>
       </c>
-      <c r="B71" s="62" t="s">
+      <c r="B73" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="C71" s="28"/>
-    </row>
-    <row r="72" spans="1:10" s="28" customFormat="1">
-      <c r="B72" s="62"/>
-      <c r="C72" s="62"/>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="4" t="s">
+      <c r="C73" s="28"/>
+    </row>
+    <row r="74" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="62"/>
+      <c r="C74" s="62"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="32" t="s">
+      <c r="B75" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="C73" s="58" t="s">
+      <c r="C75" s="58" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="28" customFormat="1">
-      <c r="D74"/>
-      <c r="E74"/>
-      <c r="F74"/>
-      <c r="G74"/>
-      <c r="H74"/>
-      <c r="I74"/>
-    </row>
-    <row r="75" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A75" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C75" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="D75"/>
-      <c r="E75"/>
-      <c r="F75"/>
-      <c r="G75"/>
-      <c r="H75"/>
-      <c r="I75"/>
-    </row>
-    <row r="76" spans="1:10" s="28" customFormat="1">
-      <c r="A76" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B76" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C76"/>
+    <row r="76" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D76"/>
       <c r="E76"/>
       <c r="F76"/>
@@ -2551,125 +2556,126 @@
       <c r="H76"/>
       <c r="I76"/>
     </row>
-    <row r="77" spans="1:10">
-      <c r="A77" s="28" t="s">
+    <row r="77" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+      <c r="H77"/>
+      <c r="I77"/>
+    </row>
+    <row r="78" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B77" s="28" t="s">
+      <c r="B79" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="J77" s="28"/>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="J78" s="28"/>
-    </row>
-    <row r="79" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A79" s="24" t="s">
+      <c r="J79" s="28"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J80" s="28"/>
+    </row>
+    <row r="81" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B81" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C79" s="29" t="s">
+      <c r="C81" s="29" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="28" customFormat="1">
-      <c r="A80" s="28" t="s">
+    <row r="82" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C80"/>
-    </row>
-    <row r="81" spans="1:10">
-      <c r="A81" s="28"/>
-      <c r="B81" s="28"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="28"/>
-      <c r="H81" s="28"/>
-      <c r="I81" s="28"/>
-      <c r="J81" s="28"/>
-    </row>
-    <row r="82" spans="1:10" s="28" customFormat="1">
-      <c r="A82" s="27" t="s">
+      <c r="C82"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="28"/>
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="28"/>
+      <c r="I83" s="28"/>
+      <c r="J83" s="28"/>
+    </row>
+    <row r="84" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B82" s="26"/>
-      <c r="C82"/>
-      <c r="D82"/>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-      <c r="H82"/>
-      <c r="I82"/>
-    </row>
-    <row r="83" spans="1:10" ht="15">
-      <c r="A83" s="28" t="s">
+      <c r="B84" s="26"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84"/>
+    </row>
+    <row r="85" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B83" s="28"/>
-      <c r="C83" s="63" t="s">
+      <c r="B85" s="28"/>
+      <c r="C85" s="63" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="28" customFormat="1">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-    </row>
-    <row r="85" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A85" s="28" t="s">
+    <row r="86" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86"/>
+    </row>
+    <row r="87" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B87" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="52" t="s">
+      <c r="C87" s="52" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A86" s="28" t="s">
+    <row r="88" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B86" s="30" t="s">
+      <c r="B88" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C86" s="45" t="s">
+      <c r="C88" s="45" t="s">
         <v>167</v>
-      </c>
-      <c r="D86"/>
-      <c r="E86"/>
-      <c r="F86"/>
-      <c r="G86"/>
-      <c r="H86"/>
-      <c r="I86"/>
-    </row>
-    <row r="87" spans="1:10" ht="15">
-      <c r="A87" t="s">
-        <v>131</v>
-      </c>
-      <c r="B87" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C87" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="D87" s="28"/>
-      <c r="E87" s="28"/>
-      <c r="F87" s="28"/>
-      <c r="G87" s="28"/>
-      <c r="H87" s="28"/>
-      <c r="I87" s="28"/>
-    </row>
-    <row r="88" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A88" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="B88" s="34" t="s">
-        <v>18</v>
       </c>
       <c r="D88"/>
       <c r="E88"/>
@@ -2678,14 +2684,16 @@
       <c r="H88"/>
       <c r="I88"/>
     </row>
-    <row r="89" spans="1:10" ht="15">
-      <c r="A89" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B89" s="38" t="s">
+    <row r="89" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>131</v>
+      </c>
+      <c r="B89" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C89" s="28"/>
+      <c r="C89" s="45" t="s">
+        <v>166</v>
+      </c>
       <c r="D89" s="28"/>
       <c r="E89" s="28"/>
       <c r="F89" s="28"/>
@@ -2693,652 +2701,700 @@
       <c r="H89" s="28"/>
       <c r="I89" s="28"/>
     </row>
-    <row r="90" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A90" t="s">
-        <v>57</v>
-      </c>
-      <c r="B90" s="38" t="s">
+    <row r="90" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90" s="34" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A91" t="s">
-        <v>110</v>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+    </row>
+    <row r="91" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="B91" s="38" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="15">
-      <c r="A92" s="28" t="s">
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="28"/>
+      <c r="H91" s="28"/>
+      <c r="I91" s="28"/>
+    </row>
+    <row r="92" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>110</v>
+      </c>
+      <c r="B93" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B92" s="63" t="s">
+      <c r="B94" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="J92" s="28"/>
-    </row>
-    <row r="93" spans="1:10" s="28" customFormat="1"/>
-    <row r="94" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A94" s="28" t="s">
+      <c r="J94" s="28"/>
+    </row>
+    <row r="95" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B95" s="63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="97" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B97" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="53" t="s">
+      <c r="C97" s="53" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="95" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A95" s="28" t="s">
+    <row r="98" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="28" t="s">
         <v>106</v>
-      </c>
-      <c r="B95" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C95" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="D95"/>
-      <c r="E95"/>
-      <c r="F95"/>
-      <c r="G95"/>
-      <c r="H95"/>
-      <c r="I95"/>
-    </row>
-    <row r="96" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A96" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B96" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C96" s="64" t="s">
-        <v>208</v>
-      </c>
-      <c r="D96"/>
-      <c r="E96"/>
-      <c r="F96"/>
-      <c r="G96"/>
-      <c r="H96"/>
-      <c r="I96"/>
-    </row>
-    <row r="97" spans="1:10" s="28" customFormat="1">
-      <c r="A97" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B97" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D97"/>
-      <c r="E97"/>
-      <c r="F97"/>
-      <c r="G97"/>
-      <c r="H97"/>
-      <c r="I97"/>
-    </row>
-    <row r="98" spans="1:10">
-      <c r="A98" s="28" t="s">
-        <v>123</v>
       </c>
       <c r="B98" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="28"/>
-      <c r="F98" s="28"/>
-      <c r="G98" s="28"/>
-      <c r="H98" s="28"/>
-      <c r="I98" s="28"/>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="A99" t="s">
-        <v>60</v>
+      <c r="C98" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98"/>
+      <c r="G98"/>
+      <c r="H98"/>
+      <c r="I98"/>
+    </row>
+    <row r="99" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="B99" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
-      <c r="E99" s="28"/>
-      <c r="F99" s="28"/>
-      <c r="G99" s="28"/>
-      <c r="H99" s="28"/>
-      <c r="I99" s="28"/>
-      <c r="J99" s="28"/>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="A100" t="s">
-        <v>109</v>
+      <c r="C99" s="64" t="s">
+        <v>208</v>
+      </c>
+      <c r="D99"/>
+      <c r="E99"/>
+      <c r="F99"/>
+      <c r="G99"/>
+      <c r="H99"/>
+      <c r="I99"/>
+    </row>
+    <row r="100" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="28"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="28"/>
-      <c r="I100" s="28"/>
-      <c r="J100" s="28"/>
-    </row>
-    <row r="101" spans="1:10" s="28" customFormat="1">
-      <c r="A101" t="s">
-        <v>122</v>
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100"/>
+      <c r="G100"/>
+      <c r="H100"/>
+      <c r="I100"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="28" t="s">
+        <v>123</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" s="28" customFormat="1"/>
-    <row r="103" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A103" s="28" t="s">
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="28"/>
+      <c r="G101" s="28"/>
+      <c r="H101" s="28"/>
+      <c r="I101" s="28"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>60</v>
+      </c>
+      <c r="B102" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="28"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="28"/>
+      <c r="I102" s="28"/>
+      <c r="J102" s="28"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>109</v>
+      </c>
+      <c r="B103" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="28"/>
+      <c r="G103" s="28"/>
+      <c r="H103" s="28"/>
+      <c r="I103" s="28"/>
+      <c r="J103" s="28"/>
+    </row>
+    <row r="104" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>122</v>
+      </c>
+      <c r="B104" s="28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="106" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B106" t="s">
         <v>21</v>
       </c>
-      <c r="C103" s="49" t="s">
+      <c r="C106" s="49" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="A104" t="s">
+    <row r="107" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>114</v>
-      </c>
-      <c r="B104" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C104" s="50" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="15">
-      <c r="A105" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B105" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C105" s="51" t="s">
-        <v>184</v>
-      </c>
-      <c r="J105" s="28"/>
-    </row>
-    <row r="106" spans="1:10" ht="15">
-      <c r="A106" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B106" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C106" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="J106" s="28"/>
-    </row>
-    <row r="107" spans="1:10" ht="15">
-      <c r="A107" t="s">
-        <v>64</v>
       </c>
       <c r="B107" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C107" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="J107" s="28"/>
-    </row>
-    <row r="108" spans="1:10">
-      <c r="A108" t="s">
-        <v>74</v>
+      <c r="C107" s="50" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A108" s="28" t="s">
+        <v>115</v>
       </c>
       <c r="B108" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D108" s="28"/>
-      <c r="E108" s="28"/>
-      <c r="F108" s="28"/>
-      <c r="G108" s="28"/>
-      <c r="H108" s="28"/>
-      <c r="I108" s="28"/>
+      <c r="C108" s="51" t="s">
+        <v>184</v>
+      </c>
       <c r="J108" s="28"/>
     </row>
-    <row r="109" spans="1:10">
-      <c r="A109" s="28"/>
-      <c r="B109" s="28"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
-      <c r="E109" s="28"/>
-      <c r="F109" s="28"/>
-      <c r="G109" s="28"/>
-      <c r="H109" s="28"/>
-      <c r="I109" s="28"/>
+    <row r="109" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C109" s="45" t="s">
+        <v>171</v>
+      </c>
       <c r="J109" s="28"/>
     </row>
-    <row r="110" spans="1:10" ht="15">
-      <c r="A110" s="28" t="s">
+    <row r="110" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>64</v>
+      </c>
+      <c r="B110" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C110" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="J110" s="28"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>74</v>
+      </c>
+      <c r="B111" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" s="28"/>
+      <c r="E111" s="28"/>
+      <c r="F111" s="28"/>
+      <c r="G111" s="28"/>
+      <c r="H111" s="28"/>
+      <c r="I111" s="28"/>
+      <c r="J111" s="28"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="28"/>
+      <c r="B112" s="28"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="28"/>
+      <c r="F112" s="28"/>
+      <c r="G112" s="28"/>
+      <c r="H112" s="28"/>
+      <c r="I112" s="28"/>
+      <c r="J112" s="28"/>
+    </row>
+    <row r="113" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C110" s="61" t="s">
+      <c r="C113" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="J110" s="28"/>
-    </row>
-    <row r="111" spans="1:10" ht="15">
-      <c r="A111" s="28" t="s">
+      <c r="J113" s="28"/>
+    </row>
+    <row r="114" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B111" s="28"/>
-      <c r="C111" s="61" t="s">
+      <c r="B114" s="28"/>
+      <c r="C114" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="J111" s="28"/>
-    </row>
-    <row r="112" spans="1:10" ht="15">
-      <c r="A112" s="28" t="s">
+      <c r="J114" s="28"/>
+    </row>
+    <row r="115" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="B112" s="28"/>
-      <c r="C112" s="61" t="s">
+      <c r="B115" s="28"/>
+      <c r="C115" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="J112" s="28"/>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="B113" s="28"/>
-      <c r="C113" s="28"/>
-      <c r="J113" s="28"/>
-    </row>
-    <row r="114" spans="1:10">
-      <c r="A114" s="28" t="s">
+      <c r="J115" s="28"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B116" s="28"/>
+      <c r="C116" s="28"/>
+      <c r="J116" s="28"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" s="28" t="s">
         <v>113</v>
-      </c>
-      <c r="B114" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="J114" s="28"/>
-    </row>
-    <row r="115" spans="1:10">
-      <c r="A115" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="B115" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="J115" s="28"/>
-    </row>
-    <row r="116" spans="1:10">
-      <c r="A116" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B116" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="J116" s="28"/>
-    </row>
-    <row r="117" spans="1:10">
-      <c r="A117" s="28" t="s">
-        <v>92</v>
       </c>
       <c r="B117" s="28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" ht="15">
+      <c r="J117" s="28"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="28" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="B118" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C118" s="45" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="15">
+      <c r="J118" s="28"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="28" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="B119" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C119" s="45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="15">
+      <c r="J119" s="28"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="28" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="B120" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C120" s="45" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="15">
-      <c r="A121" t="s">
-        <v>75</v>
+    </row>
+    <row r="121" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="28" t="s">
+        <v>147</v>
       </c>
       <c r="B121" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C121" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="J121" s="28"/>
-    </row>
-    <row r="122" spans="1:10">
-      <c r="A122" t="s">
-        <v>67</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="28" t="s">
+        <v>126</v>
       </c>
       <c r="B122" s="28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="123" spans="1:10">
-      <c r="A123" t="s">
-        <v>68</v>
+      <c r="C122" s="45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="28" t="s">
+        <v>117</v>
       </c>
       <c r="B123" s="28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="124" spans="1:10">
-      <c r="A124" s="28" t="s">
-        <v>79</v>
+      <c r="C123" s="45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>75</v>
       </c>
       <c r="B124" s="28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" ht="15">
-      <c r="A125" s="28" t="s">
-        <v>80</v>
+      <c r="C124" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="J124" s="28"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>67</v>
       </c>
       <c r="B125" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C125" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="J125" s="28"/>
-    </row>
-    <row r="126" spans="1:10" ht="15">
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="B126" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C126" s="46"/>
-      <c r="J126" s="28"/>
-    </row>
-    <row r="127" spans="1:10" ht="15">
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="28" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B127" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C127" s="45"/>
-      <c r="J127" s="28"/>
-    </row>
-    <row r="128" spans="1:10">
-      <c r="A128" t="s">
-        <v>85</v>
+    </row>
+    <row r="128" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="28" t="s">
+        <v>80</v>
       </c>
       <c r="B128" s="28" t="s">
         <v>22</v>
       </c>
+      <c r="C128" s="45" t="s">
+        <v>178</v>
+      </c>
       <c r="J128" s="28"/>
     </row>
-    <row r="129" spans="1:10" ht="15">
-      <c r="C129" s="45"/>
+    <row r="129" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>107</v>
+      </c>
+      <c r="B129" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C129" s="46"/>
       <c r="J129" s="28"/>
     </row>
-    <row r="130" spans="1:10" ht="15">
-      <c r="A130" t="s">
+    <row r="130" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B130" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C130" s="45"/>
+      <c r="J130" s="28"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>85</v>
+      </c>
+      <c r="B131" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J131" s="28"/>
+    </row>
+    <row r="132" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B132" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C133" s="45"/>
+      <c r="J133" s="28"/>
+    </row>
+    <row r="134" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>81</v>
       </c>
-      <c r="B130" s="37" t="s">
+      <c r="B134" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C130" s="48" t="s">
+      <c r="C134" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="J130" s="28"/>
-    </row>
-    <row r="131" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="B131" s="48"/>
-      <c r="C131" s="48" t="s">
+      <c r="J134" s="28"/>
+    </row>
+    <row r="135" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B135" s="48"/>
+      <c r="C135" s="48" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
-      <c r="J132" s="28"/>
-    </row>
-    <row r="133" spans="1:10" ht="15">
-      <c r="A133" t="s">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J136" s="28"/>
+    </row>
+    <row r="137" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>120</v>
       </c>
-      <c r="B133" s="36" t="s">
+      <c r="B137" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C133" s="47" t="s">
+      <c r="C137" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="J133" s="28"/>
-    </row>
-    <row r="134" spans="1:10" ht="15">
-      <c r="A134" t="s">
+      <c r="J137" s="28"/>
+    </row>
+    <row r="138" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>121</v>
       </c>
-      <c r="B134" s="38" t="s">
+      <c r="B138" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="J134" s="28"/>
-    </row>
-    <row r="135" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="B135" s="63"/>
-    </row>
-    <row r="136" spans="1:10" ht="15">
-      <c r="A136" t="s">
+      <c r="J138" s="28"/>
+    </row>
+    <row r="139" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B139" s="63"/>
+    </row>
+    <row r="140" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>108</v>
       </c>
-      <c r="B136" s="38" t="s">
+      <c r="B140" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="C136" s="64" t="s">
+      <c r="C140" s="64" t="s">
         <v>202</v>
       </c>
-      <c r="J136" s="28"/>
-    </row>
-    <row r="137" spans="1:10" ht="15">
-      <c r="A137" s="28" t="s">
+      <c r="J140" s="28"/>
+    </row>
+    <row r="141" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A141" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B137" s="63" t="s">
+      <c r="B141" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="C137" s="64" t="s">
+      <c r="C141" s="64" t="s">
         <v>203</v>
       </c>
-      <c r="J137" s="28"/>
-    </row>
-    <row r="138" spans="1:10" ht="15">
-      <c r="B138" s="63" t="s">
+      <c r="J141" s="28"/>
+    </row>
+    <row r="142" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B142" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="C138" s="64" t="s">
+      <c r="C142" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="J138" s="28"/>
-    </row>
-    <row r="139" spans="1:10" ht="15">
-      <c r="A139" t="s">
+      <c r="J142" s="28"/>
+    </row>
+    <row r="143" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>149</v>
       </c>
-      <c r="B139" s="63" t="s">
+      <c r="B143" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="J139" s="28"/>
-    </row>
-    <row r="140" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="C140" s="64"/>
-    </row>
-    <row r="141" spans="1:10" ht="15">
-      <c r="A141" s="28" t="s">
+      <c r="J143" s="28"/>
+    </row>
+    <row r="144" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="C144" s="64"/>
+    </row>
+    <row r="145" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B145" t="s">
         <v>158</v>
       </c>
-      <c r="C141" s="55" t="s">
+      <c r="C145" s="55" t="s">
         <v>188</v>
       </c>
-      <c r="J141" s="28"/>
-    </row>
-    <row r="142" spans="1:10" ht="15">
-      <c r="A142" s="28" t="s">
+      <c r="J145" s="28"/>
+    </row>
+    <row r="146" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B142" s="28" t="s">
+      <c r="B146" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="C142" s="55" t="s">
+      <c r="C146" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="J142" s="28"/>
-    </row>
-    <row r="143" spans="1:10" ht="15">
-      <c r="A143" t="s">
+      <c r="J146" s="28"/>
+    </row>
+    <row r="147" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>112</v>
       </c>
-      <c r="B143" s="28" t="s">
+      <c r="B147" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="C143" s="55" t="s">
+      <c r="C147" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="J143" s="28"/>
-    </row>
-    <row r="144" spans="1:10" ht="15">
-      <c r="B144" s="28" t="s">
+      <c r="J147" s="28"/>
+    </row>
+    <row r="148" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B148" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="C144" s="55" t="s">
+      <c r="C148" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="J144" s="28"/>
-    </row>
-    <row r="145" spans="1:10" s="28" customFormat="1" ht="15">
-      <c r="C145" s="55"/>
-    </row>
-    <row r="146" spans="1:10" ht="15">
-      <c r="A146" t="s">
+      <c r="J148" s="28"/>
+    </row>
+    <row r="149" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="C149" s="55"/>
+    </row>
+    <row r="150" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>78</v>
       </c>
-      <c r="B146" s="65" t="s">
+      <c r="B150" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="C146" s="64" t="s">
+      <c r="C150" s="64" t="s">
         <v>210</v>
       </c>
-      <c r="J146" s="28"/>
-    </row>
-    <row r="147" spans="1:10">
-      <c r="A147" s="28" t="s">
+      <c r="J150" s="28"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A151" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B147" s="65" t="s">
+      <c r="B151" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="J147" s="28"/>
-    </row>
-    <row r="148" spans="1:10">
-      <c r="B148" s="40"/>
-      <c r="J148" s="28"/>
-    </row>
-    <row r="149" spans="1:10" s="16" customFormat="1" ht="15">
-      <c r="A149" s="28" t="s">
+      <c r="J151" s="28"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B152" s="40"/>
+      <c r="J152" s="28"/>
+    </row>
+    <row r="153" spans="1:10" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A153" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="B149" s="63" t="s">
+      <c r="B153" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="C149" s="63" t="s">
+      <c r="C153" s="63" t="s">
         <v>205</v>
       </c>
-      <c r="E149" s="16" t="s">
+      <c r="E153" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="F149"/>
-      <c r="J149" s="28"/>
-    </row>
-    <row r="150" spans="1:10" ht="15">
-      <c r="A150" s="28" t="s">
+      <c r="F153"/>
+      <c r="J153" s="28"/>
+    </row>
+    <row r="154" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A154" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B150" s="63" t="s">
+      <c r="B154" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="C150" s="56" t="s">
+      <c r="C154" s="56" t="s">
         <v>192</v>
       </c>
-      <c r="J150" s="28"/>
-    </row>
-    <row r="151" spans="1:10" ht="15">
-      <c r="A151" s="28" t="s">
+      <c r="J154" s="28"/>
+    </row>
+    <row r="155" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A155" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="B151" s="63" t="s">
+      <c r="B155" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="C151" s="28"/>
-    </row>
-    <row r="152" spans="1:10" ht="15">
-      <c r="A152" s="28" t="s">
+      <c r="C155" s="28"/>
+    </row>
+    <row r="156" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A156" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C152" s="57" t="s">
+      <c r="C156" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E156" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
-      <c r="J153" s="28"/>
-    </row>
-    <row r="154" spans="1:10">
-      <c r="A154" t="s">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J157" s="28"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>62</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E158" t="s">
         <v>209</v>
       </c>
-      <c r="J154" s="28"/>
-    </row>
-    <row r="155" spans="1:10">
-      <c r="A155" s="28" t="s">
+      <c r="J158" s="28"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A159" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E155" s="28" t="s">
+      <c r="E159" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="J155" s="28"/>
-    </row>
-    <row r="156" spans="1:10">
-      <c r="J156" s="28"/>
+      <c r="J159" s="28"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>216</v>
+      </c>
+      <c r="J160" s="28"/>
     </row>
   </sheetData>
-  <sortState ref="J1:J155">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J1:J159">
     <sortCondition ref="J1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3352,16 +3408,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -3381,7 +3437,7 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -3412,16 +3468,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3447,7 +3503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update To Australia inventory scaling 1. Update to scaling map 2. Now only scale to years 2001-2018 due to jump between 2000 and 2001
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Australia_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Australia_scaling_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/mappings/scaling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB58DFF-A9E3-2740-97F4-B04C3F765608}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC34626-067D-AE47-9454-C6FAD5923D8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="5020" windowWidth="17340" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8860" yWindow="2180" windowWidth="17340" windowHeight="12980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="219">
   <si>
     <t>iso</t>
   </si>
@@ -690,9 +690,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1156,182 +1163,182 @@
   </borders>
   <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1349,55 +1356,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="45"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="175">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1878,11 +1886,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B141" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A153" sqref="A153"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3471,8 +3479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3504,10 +3512,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="66" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="19" t="s">
@@ -3519,13 +3527,15 @@
       <c r="E2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="66" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Scaling Mapping for Australia
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Australia_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Australia_scaling_mapping.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC34626-067D-AE47-9454-C6FAD5923D8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D9F48E-251A-E64E-9CE0-B2686BB1FAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="2180" windowWidth="17340" windowHeight="12980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10920" yWindow="8620" windowWidth="17340" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="219">
   <si>
     <t>iso</t>
   </si>
@@ -1884,13 +1890,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J160"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2756,7 +2762,7 @@
     </row>
     <row r="94" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="28" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="B94" s="63" t="s">
         <v>18</v>
@@ -2764,12 +2770,7 @@
       <c r="J94" s="28"/>
     </row>
     <row r="95" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="B95" s="63" t="s">
-        <v>18</v>
-      </c>
+      <c r="B95" s="63"/>
     </row>
     <row r="96" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="97" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2899,8 +2900,8 @@
       </c>
     </row>
     <row r="107" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>114</v>
+      <c r="A107" s="28" t="s">
+        <v>115</v>
       </c>
       <c r="B107" s="28" t="s">
         <v>21</v>
@@ -2911,7 +2912,7 @@
     </row>
     <row r="108" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="28" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="B108" s="28" t="s">
         <v>21</v>
@@ -2922,8 +2923,8 @@
       <c r="J108" s="28"/>
     </row>
     <row r="109" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="28" t="s">
-        <v>66</v>
+      <c r="A109" t="s">
+        <v>64</v>
       </c>
       <c r="B109" s="28" t="s">
         <v>21</v>
@@ -2933,25 +2934,17 @@
       </c>
       <c r="J109" s="28"/>
     </row>
-    <row r="110" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B110" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C110" s="45" t="s">
-        <v>175</v>
-      </c>
       <c r="J110" s="28"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>74</v>
-      </c>
-      <c r="B111" s="28" t="s">
-        <v>21</v>
-      </c>
+      <c r="B111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
       <c r="F111" s="28"/>
@@ -3160,249 +3153,276 @@
       </c>
     </row>
     <row r="133" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C133" s="45"/>
+      <c r="A133" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B133" t="s">
+        <v>22</v>
+      </c>
+      <c r="C133" s="45" t="s">
+        <v>175</v>
+      </c>
       <c r="J133" s="28"/>
     </row>
-    <row r="134" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>81</v>
-      </c>
-      <c r="B134" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C134" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="J134" s="28"/>
+        <v>114</v>
+      </c>
+      <c r="B134" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C134" s="63"/>
     </row>
     <row r="135" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B135" s="48"/>
-      <c r="C135" s="48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J136" s="28"/>
+      <c r="A135" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B135" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C135" s="63"/>
+    </row>
+    <row r="136" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="C136" s="63"/>
     </row>
     <row r="137" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>120</v>
-      </c>
-      <c r="B137" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C137" s="47" t="s">
-        <v>179</v>
+        <v>81</v>
+      </c>
+      <c r="B137" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C137" s="48" t="s">
+        <v>180</v>
       </c>
       <c r="J137" s="28"/>
     </row>
-    <row r="138" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>121</v>
-      </c>
-      <c r="B138" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="J138" s="28"/>
-    </row>
-    <row r="139" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B139" s="63"/>
+    <row r="138" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B138" s="48"/>
+      <c r="C138" s="48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J139" s="28"/>
     </row>
     <row r="140" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>108</v>
-      </c>
-      <c r="B140" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="C140" s="64" t="s">
-        <v>202</v>
+        <v>120</v>
+      </c>
+      <c r="B140" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C140" s="47" t="s">
+        <v>179</v>
       </c>
       <c r="J140" s="28"/>
     </row>
     <row r="141" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A141" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B141" s="63" t="s">
-        <v>201</v>
-      </c>
-      <c r="C141" s="64" t="s">
-        <v>203</v>
+      <c r="A141" t="s">
+        <v>121</v>
+      </c>
+      <c r="B141" s="38" t="s">
+        <v>14</v>
       </c>
       <c r="J141" s="28"/>
     </row>
-    <row r="142" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B142" s="63" t="s">
-        <v>201</v>
-      </c>
-      <c r="C142" s="64" t="s">
-        <v>204</v>
-      </c>
-      <c r="J142" s="28"/>
+    <row r="142" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B142" s="63"/>
     </row>
     <row r="143" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>108</v>
+      </c>
+      <c r="B143" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="C143" s="64" t="s">
+        <v>202</v>
+      </c>
+      <c r="J143" s="28"/>
+    </row>
+    <row r="144" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B144" s="63" t="s">
+        <v>201</v>
+      </c>
+      <c r="C144" s="64" t="s">
+        <v>203</v>
+      </c>
+      <c r="J144" s="28"/>
+    </row>
+    <row r="145" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>149</v>
       </c>
-      <c r="B143" s="63" t="s">
+      <c r="B145" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="J143" s="28"/>
-    </row>
-    <row r="144" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="C144" s="64"/>
-    </row>
-    <row r="145" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A145" s="28" t="s">
+      <c r="C145" s="64" t="s">
+        <v>204</v>
+      </c>
+      <c r="J145" s="28"/>
+    </row>
+    <row r="146" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="28"/>
+      <c r="B146" s="63"/>
+      <c r="J146" s="28"/>
+    </row>
+    <row r="147" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B147" s="63"/>
+    </row>
+    <row r="148" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A148" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B145" t="s">
-        <v>158</v>
-      </c>
-      <c r="C145" s="55" t="s">
-        <v>188</v>
-      </c>
-      <c r="J145" s="28"/>
-    </row>
-    <row r="146" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A146" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="B146" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C146" s="55" t="s">
-        <v>189</v>
-      </c>
-      <c r="J146" s="28"/>
-    </row>
-    <row r="147" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>112</v>
-      </c>
-      <c r="B147" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="C147" s="55" t="s">
-        <v>190</v>
-      </c>
-      <c r="J147" s="28"/>
-    </row>
-    <row r="148" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="B148" s="28" t="s">
         <v>158</v>
       </c>
       <c r="C148" s="55" t="s">
-        <v>191</v>
-      </c>
-      <c r="J148" s="28"/>
-    </row>
-    <row r="149" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="C149" s="55"/>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A149" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B149" t="s">
+        <v>158</v>
+      </c>
+      <c r="C149" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="J149" s="28"/>
     </row>
     <row r="150" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
+        <v>112</v>
+      </c>
+      <c r="B150" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C150" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="J150" s="28"/>
+    </row>
+    <row r="151" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="B151" s="28"/>
+      <c r="C151" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="J151" s="28"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A152" s="28"/>
+      <c r="B152" s="28"/>
+      <c r="J152" s="28"/>
+    </row>
+    <row r="153" spans="1:10" s="28" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>78</v>
       </c>
-      <c r="B150" s="65" t="s">
+      <c r="B153" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="C150" s="64" t="s">
-        <v>210</v>
-      </c>
-      <c r="J150" s="28"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A151" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B151" s="65" t="s">
-        <v>211</v>
-      </c>
-      <c r="J151" s="28"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B152" s="40"/>
-      <c r="J152" s="28"/>
-    </row>
-    <row r="153" spans="1:10" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A153" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="B153" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="C153" s="63" t="s">
-        <v>205</v>
-      </c>
-      <c r="E153" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="F153"/>
-      <c r="J153" s="28"/>
+      <c r="C153" s="55"/>
     </row>
     <row r="154" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="B154" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="C154" s="56" t="s">
-        <v>192</v>
+        <v>82</v>
+      </c>
+      <c r="B154" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="C154" s="64" t="s">
+        <v>210</v>
       </c>
       <c r="J154" s="28"/>
     </row>
-    <row r="155" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A155" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B155" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="C155" s="28"/>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B155" s="40"/>
+      <c r="J155" s="28"/>
     </row>
     <row r="156" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C156" s="57" t="s">
-        <v>193</v>
-      </c>
-      <c r="E156" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="B156" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="J156" s="28"/>
+    </row>
+    <row r="157" spans="1:10" s="16" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A157" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B157" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="C157" s="63" t="s">
+        <v>205</v>
+      </c>
+      <c r="E157" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="F157"/>
       <c r="J157" s="28"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>62</v>
-      </c>
-      <c r="E158" t="s">
-        <v>209</v>
+    <row r="158" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A158" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B158" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="C158" s="56" t="s">
+        <v>192</v>
       </c>
       <c r="J158" s="28"/>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C159" s="28"/>
+    </row>
+    <row r="160" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C160" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="E160" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>62</v>
+      </c>
+      <c r="J161" s="28"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A162" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E159" s="28" t="s">
+      <c r="E162" t="s">
         <v>209</v>
       </c>
-      <c r="J159" s="28"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+      <c r="J162" s="28"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>216</v>
       </c>
-      <c r="J160" s="28"/>
+      <c r="E163" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="J163" s="28"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J164" s="28"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J1:J159">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J1:J161">
     <sortCondition ref="J1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3479,7 +3499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>